<commit_message>
chore (mock-data.xlsx): label year quarter columns as "yq"
</commit_message>
<xml_diff>
--- a/mock-data.xlsx
+++ b/mock-data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stoja\fim-shiny\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E967F3E-2ADC-463C-A99F-5398046B458A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED0A7D76-7BCC-4DA5-98FD-9259C2BD95E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-3390" windowWidth="29040" windowHeight="15720" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="52">
   <si>
     <t>2024 Q1</t>
   </si>
@@ -194,6 +194,9 @@
   </si>
   <si>
     <t>for transfers</t>
+  </si>
+  <si>
+    <t>yq</t>
   </si>
 </sst>
 </file>
@@ -520,7 +523,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:E40"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -536,6 +541,9 @@
       </c>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>51</v>
+      </c>
       <c r="C3" t="s">
         <v>42</v>
       </c>
@@ -993,7 +1001,7 @@
   <dimension ref="B2:E40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1010,6 +1018,9 @@
       </c>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>51</v>
+      </c>
       <c r="C3" t="str">
         <f>h.itemized!C3</f>
         <v>purchases</v>
@@ -1299,7 +1310,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C78E83D-0D79-4FC2-BBB2-BDA3D59A7780}">
   <dimension ref="B2:C40"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -1309,6 +1322,9 @@
       </c>
     </row>
     <row r="3" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>51</v>
+      </c>
       <c r="C3" t="s">
         <v>37</v>
       </c>
@@ -1592,7 +1608,7 @@
   <dimension ref="B2:C40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E33" sqref="E33"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1603,6 +1619,9 @@
       </c>
     </row>
     <row r="3" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>51</v>
+      </c>
       <c r="C3" t="str">
         <f>h.macro!C3</f>
         <v>potgdp</v>
@@ -2049,12 +2068,15 @@
   <dimension ref="B3:E40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I21" sqref="I21"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="3" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>51</v>
+      </c>
       <c r="C3" t="str">
         <f>h.itemized!C3</f>
         <v>purchases</v>

</xml_diff>